<commit_message>
Updating code for simulink and MATLAB lectures
</commit_message>
<xml_diff>
--- a/Code/AY 2020_21/05 Tables/mpg.xlsx
+++ b/Code/AY 2020_21/05 Tables/mpg.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimd/Dropbox/Lectures GITHUB/CT248/Code/AY 2020_21/05 Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{204A8D60-98D3-F740-925E-358D66D6A2C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFCEB88-0678-0046-BAA1-74A875ACFCBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="2800" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="2260" yWindow="520" windowWidth="31800" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mpg" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mpg!$A$1:$K$235</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -286,7 +300,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1120,12 +1134,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
+      <selection sqref="A1:K1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="5.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -9353,6 +9382,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K235" xr:uid="{80140A50-25E9-3B41-8469-81E7DE89631C}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>